<commit_message>
The experiment redone fully
</commit_message>
<xml_diff>
--- a/experiments/experiments_featureselection/bikes_regr_results.xlsx
+++ b/experiments/experiments_featureselection/bikes_regr_results.xlsx
@@ -1641,10 +1641,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1655,10 +1657,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1669,10 +1673,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1683,10 +1689,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1697,10 +1705,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1711,10 +1721,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1725,10 +1737,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1739,10 +1753,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1757,10 +1773,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t>47.178</t>
     </r>
@@ -1771,10 +1789,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1785,10 +1805,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1799,10 +1821,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1813,10 +1837,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1827,10 +1853,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1841,10 +1869,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1855,10 +1885,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1869,10 +1901,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1883,10 +1917,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1897,10 +1933,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1911,10 +1949,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1925,10 +1965,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1939,10 +1981,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1953,10 +1997,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1970,10 +2016,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1984,10 +2032,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1998,10 +2048,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -2012,10 +2064,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -2026,10 +2080,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -2040,10 +2096,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -2054,10 +2112,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -2068,10 +2128,12 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -2083,17 +2145,289 @@
     </r>
     <r>
       <rPr>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t>50.079</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>36.883</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>52.363</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>38.819</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>50.962</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>36.623</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>52.142</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>29.353</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>56.918</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>38.979</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>49.079</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>40.285</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>50.708</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>39.224</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>50.734</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>39.111</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>51.03</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="false"/>
+        <i val="false"/>
+        <u val="none"/>
+        <rFont val="Segoe UI"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>56.183</t>
+    </r>
+    <r>
+      <rPr>
         <rFont val="Segoe UI"/>
         <sz val="9"/>
         <color rgb="FF000000"/>
         <vertAlign val="baseline"/>
       </rPr>
-      <t>50.079</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>36.883</t>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>34.581</t>
     </r>
     <r>
       <rPr>
@@ -2107,7 +2441,7 @@
   </si>
   <si>
     <r>
-      <t>52.363</t>
+      <t>39.311</t>
     </r>
     <r>
       <rPr>
@@ -2121,7 +2455,7 @@
   </si>
   <si>
     <r>
-      <t>38.819</t>
+      <t>50.184</t>
     </r>
     <r>
       <rPr>
@@ -2135,7 +2469,7 @@
   </si>
   <si>
     <r>
-      <t>50.962</t>
+      <t>38.577</t>
     </r>
     <r>
       <rPr>
@@ -2149,7 +2483,7 @@
   </si>
   <si>
     <r>
-      <t>36.623</t>
+      <t>50.929</t>
     </r>
     <r>
       <rPr>
@@ -2163,7 +2497,7 @@
   </si>
   <si>
     <r>
-      <t>52.142</t>
+      <t>39.588</t>
     </r>
     <r>
       <rPr>
@@ -2177,7 +2511,7 @@
   </si>
   <si>
     <r>
-      <t>29.353</t>
+      <t>50.723</t>
     </r>
     <r>
       <rPr>
@@ -2190,8 +2524,11 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>56.918</t>
+    <t>38.22</t>
+  </si>
+  <si>
+    <r>
+      <t>51.413</t>
     </r>
     <r>
       <rPr>
@@ -2204,123 +2541,17 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>38.979</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>49.079</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>40.285</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>50.708</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>39.224</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>50.734</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>39.111</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>51.03</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Segoe UI"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <vertAlign val="baseline"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
+    <t>52.183</t>
+  </si>
+  <si>
+    <t>49.918</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2353,6 +2584,11 @@
       <color rgb="FF000000"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Segoe UI"/>
+      <color rgb="FF000000"/>
     </font>
     <font>
       <sz val="9"/>
@@ -3348,7 +3584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3563,8 +3799,8 @@
       <c r="F6" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>166</v>
+      <c r="G6" s="4" t="s">
+        <v>186</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>173</v>
@@ -3580,6 +3816,49 @@
       </c>
       <c r="O6" s="3" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" ht="23.25">
+      <c r="K8" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>